<commit_message>
datacapture logic change based on schema changes
</commit_message>
<xml_diff>
--- a/SampleInputFiles/sample_InProgress_Greenland.xlsx
+++ b/SampleInputFiles/sample_InProgress_Greenland.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishn\OneDrive\Desktop\MyEngineering\golocalrefactor\SampleInputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457FBC89-7A07-4A9C-AE08-EE3654C70334}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D00A9B-0554-4EA6-B945-D35C87DAB45B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="0" windowWidth="24973" windowHeight="10153" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3733" yWindow="0" windowWidth="24973" windowHeight="10153" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -1327,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA816A8A-C50A-46C0-B933-059E5986472F}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1590,7 +1590,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="19">
-        <v>42370</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
@@ -1600,7 +1600,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="19">
-        <v>42370</v>
+        <v>43101</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">

</xml_diff>